<commit_message>
add error code, change uri get user info
</commit_message>
<xml_diff>
--- a/doc/detail_design/backend/api/TRN-MiniBlog_API-Specification_Tam-V.Anh.xlsx
+++ b/doc/detail_design/backend/api/TRN-MiniBlog_API-Specification_Tam-V.Anh.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23206"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28080" windowHeight="19080" tabRatio="957" firstSheet="3" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28080" windowHeight="19080" tabRatio="957" firstSheet="3" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="23" r:id="rId1"/>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3636" uniqueCount="631">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3636" uniqueCount="632">
   <si>
     <t>Description</t>
   </si>
@@ -1865,9 +1865,6 @@
     <t>GET /v1/users/13/posts</t>
   </si>
   <si>
-    <t>GET /v1/users/13</t>
-  </si>
-  <si>
     <t>/v1/posts</t>
     <phoneticPr fontId="14"/>
   </si>
@@ -1916,10 +1913,6 @@
     <phoneticPr fontId="14"/>
   </si>
   <si>
-    <t>/v1/users/{user_id}</t>
-    <phoneticPr fontId="14"/>
-  </si>
-  <si>
     <t>/v1/users/{user_id}/posts</t>
     <phoneticPr fontId="14"/>
   </si>
@@ -1928,10 +1921,6 @@
     <phoneticPr fontId="14"/>
   </si>
   <si>
-    <t>http://{domain}/v1/users/{user_id}</t>
-    <phoneticPr fontId="14"/>
-  </si>
-  <si>
     <t xml:space="preserve">GET /v1/posts?limit=20&amp;offset=20&amp;order=date </t>
     <phoneticPr fontId="14"/>
   </si>
@@ -2321,6 +2310,22 @@
   </si>
   <si>
     <t>Can not found result by keyword</t>
+    <phoneticPr fontId="14"/>
+  </si>
+  <si>
+    <t>http://{domain}/v1/users</t>
+    <phoneticPr fontId="14"/>
+  </si>
+  <si>
+    <t>Yes</t>
+    <phoneticPr fontId="14"/>
+  </si>
+  <si>
+    <t>/v1/users</t>
+    <phoneticPr fontId="14"/>
+  </si>
+  <si>
+    <t>GET /v1/users</t>
     <phoneticPr fontId="14"/>
   </si>
 </sst>
@@ -20590,7 +20595,7 @@
               <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
               <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
             </a:rPr>
-            <a:t>GET /v1/users/user-id HTTP/1.1</a:t>
+            <a:t>GET /v1/users HTTP/1.1</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -22373,7 +22378,7 @@
         <v>439</v>
       </c>
       <c r="B2" s="144" t="s">
-        <v>600</v>
+        <v>597</v>
       </c>
       <c r="C2" s="168"/>
       <c r="D2" s="168"/>
@@ -22414,7 +22419,7 @@
         <v>122</v>
       </c>
       <c r="C4" s="291" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
       <c r="D4" s="299"/>
       <c r="E4" s="299"/>
@@ -22435,7 +22440,7 @@
         <v>123</v>
       </c>
       <c r="C5" s="291" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="D5" s="299"/>
       <c r="E5" s="299"/>
@@ -22456,7 +22461,7 @@
         <v>161</v>
       </c>
       <c r="C6" s="224" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
       <c r="D6" s="227"/>
       <c r="E6" s="227"/>
@@ -22477,7 +22482,7 @@
         <v>170</v>
       </c>
       <c r="C7" s="291" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
       <c r="D7" s="299"/>
       <c r="E7" s="299"/>
@@ -22498,7 +22503,7 @@
         <v>171</v>
       </c>
       <c r="C8" s="224" t="s">
-        <v>605</v>
+        <v>602</v>
       </c>
       <c r="D8" s="227"/>
       <c r="E8" s="227"/>
@@ -23008,7 +23013,7 @@
         <v>185</v>
       </c>
       <c r="I30" s="140" t="s">
-        <v>606</v>
+        <v>603</v>
       </c>
       <c r="J30" s="140" t="s">
         <v>137</v>
@@ -23555,7 +23560,7 @@
       </c>
       <c r="E58" s="305"/>
       <c r="F58" s="139" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
       <c r="G58" s="140" t="s">
         <v>137</v>
@@ -23573,7 +23578,7 @@
         <v>137</v>
       </c>
       <c r="L58" s="141" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="M58" s="168"/>
       <c r="N58" s="168"/>
@@ -24170,7 +24175,7 @@
         <v>161</v>
       </c>
       <c r="C6" s="164" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="D6" s="172"/>
       <c r="E6" s="172"/>
@@ -25140,7 +25145,7 @@
       </c>
       <c r="F42" s="165"/>
       <c r="G42" s="139" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="H42" s="140" t="s">
         <v>164</v>
@@ -25174,7 +25179,7 @@
       </c>
       <c r="F43" s="165"/>
       <c r="G43" s="139" t="s">
-        <v>584</v>
+        <v>581</v>
       </c>
       <c r="H43" s="140" t="s">
         <v>164</v>
@@ -26789,7 +26794,7 @@
         <v>161</v>
       </c>
       <c r="C6" s="164" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
       <c r="D6" s="172"/>
       <c r="E6" s="172"/>
@@ -27764,27 +27769,27 @@
       <c r="B44" s="310"/>
       <c r="C44" s="310"/>
       <c r="D44" s="217" t="s">
-        <v>564</v>
+        <v>561</v>
       </c>
       <c r="E44" s="216"/>
       <c r="F44" s="139" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
       <c r="G44" s="140" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
       <c r="H44" s="140"/>
       <c r="I44" s="140">
         <v>1</v>
       </c>
       <c r="J44" s="140" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
       <c r="K44" s="140" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
       <c r="L44" s="141" t="s">
-        <v>567</v>
+        <v>564</v>
       </c>
       <c r="M44" s="168"/>
       <c r="N44" s="168"/>
@@ -27795,24 +27800,24 @@
       <c r="B45" s="311"/>
       <c r="C45" s="311"/>
       <c r="D45" s="217" t="s">
-        <v>568</v>
+        <v>565</v>
       </c>
       <c r="E45" s="216"/>
       <c r="F45" s="139" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
       <c r="G45" s="140" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
       <c r="H45" s="140"/>
       <c r="I45" s="140">
         <v>1</v>
       </c>
       <c r="J45" s="140" t="s">
+        <v>563</v>
+      </c>
+      <c r="K45" s="140" t="s">
         <v>566</v>
-      </c>
-      <c r="K45" s="140" t="s">
-        <v>569</v>
       </c>
       <c r="L45" s="218" t="s">
         <v>411</v>
@@ -29241,8 +29246,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O104"/>
   <sheetViews>
-    <sheetView topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="L56" sqref="L56"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9:I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -29367,7 +29372,7 @@
         <v>161</v>
       </c>
       <c r="C6" s="164" t="s">
-        <v>532</v>
+        <v>628</v>
       </c>
       <c r="D6" s="172"/>
       <c r="E6" s="172"/>
@@ -29409,7 +29414,7 @@
         <v>171</v>
       </c>
       <c r="C8" s="164" t="s">
-        <v>28</v>
+        <v>629</v>
       </c>
       <c r="D8" s="172"/>
       <c r="E8" s="172"/>
@@ -30313,7 +30318,7 @@
       </c>
       <c r="E43" s="290"/>
       <c r="F43" s="141" t="s">
-        <v>587</v>
+        <v>584</v>
       </c>
       <c r="G43" s="140" t="s">
         <v>164</v>
@@ -30346,7 +30351,7 @@
       </c>
       <c r="E44" s="290"/>
       <c r="F44" s="141" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="G44" s="140" t="s">
         <v>164</v>
@@ -32353,7 +32358,7 @@
         <v>185</v>
       </c>
       <c r="I35" s="140" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="J35" s="76" t="s">
         <v>137</v>
@@ -32476,7 +32481,7 @@
       </c>
       <c r="E39" s="151"/>
       <c r="F39" s="139" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
       <c r="G39" s="76" t="s">
         <v>164</v>
@@ -34667,7 +34672,7 @@
       </c>
       <c r="E35" s="151"/>
       <c r="F35" s="139" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
       <c r="G35" s="76" t="s">
         <v>164</v>
@@ -35937,7 +35942,7 @@
         <v>161</v>
       </c>
       <c r="C6" s="150" t="s">
-        <v>548</v>
+        <v>545</v>
       </c>
       <c r="D6" s="153"/>
       <c r="E6" s="153"/>
@@ -36186,10 +36191,10 @@
       <c r="A17" s="66"/>
       <c r="B17" s="73"/>
       <c r="C17" s="139" t="s">
-        <v>552</v>
+        <v>549</v>
       </c>
       <c r="D17" s="141" t="s">
-        <v>553</v>
+        <v>550</v>
       </c>
       <c r="E17" s="140" t="s">
         <v>266</v>
@@ -36220,7 +36225,7 @@
         <v>299</v>
       </c>
       <c r="D18" s="141" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
       <c r="E18" s="140" t="s">
         <v>300</v>
@@ -36702,7 +36707,7 @@
       </c>
       <c r="E38" s="316"/>
       <c r="F38" s="139" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
       <c r="G38" s="76" t="s">
         <v>164</v>
@@ -36735,7 +36740,7 @@
       </c>
       <c r="E39" s="151"/>
       <c r="F39" s="139" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
       <c r="G39" s="76" t="s">
         <v>164</v>
@@ -38133,7 +38138,7 @@
         <v>161</v>
       </c>
       <c r="C6" s="150" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="D6" s="153"/>
       <c r="E6" s="153"/>
@@ -38485,10 +38490,10 @@
       <c r="A20" s="66"/>
       <c r="B20" s="327"/>
       <c r="C20" s="139" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
       <c r="D20" s="141" t="s">
-        <v>556</v>
+        <v>553</v>
       </c>
       <c r="E20" s="140" t="s">
         <v>266</v>
@@ -38503,10 +38508,10 @@
         <v>282</v>
       </c>
       <c r="I20" s="162" t="s">
-        <v>557</v>
+        <v>554</v>
       </c>
       <c r="J20" s="291" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
       <c r="K20" s="315"/>
       <c r="L20" s="316"/>
@@ -39984,7 +39989,7 @@
         <v>161</v>
       </c>
       <c r="C6" s="150" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="D6" s="153"/>
       <c r="E6" s="153"/>
@@ -40339,7 +40344,7 @@
         <v>335</v>
       </c>
       <c r="D20" s="141" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
       <c r="E20" s="140" t="s">
         <v>266</v>
@@ -41852,7 +41857,7 @@
         <v>161</v>
       </c>
       <c r="C6" s="150" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="D6" s="153"/>
       <c r="E6" s="153"/>
@@ -42042,7 +42047,7 @@
         <v>338</v>
       </c>
       <c r="D15" s="141" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
       <c r="E15" s="140" t="s">
         <v>313</v>
@@ -44718,7 +44723,7 @@
         <v>185</v>
       </c>
       <c r="I31" s="140" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
       <c r="J31" s="76" t="s">
         <v>137</v>
@@ -44808,7 +44813,7 @@
       </c>
       <c r="E34" s="151"/>
       <c r="F34" s="139" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
       <c r="G34" s="76" t="s">
         <v>164</v>
@@ -46282,7 +46287,7 @@
         <v>161</v>
       </c>
       <c r="C6" s="150" t="s">
-        <v>549</v>
+        <v>546</v>
       </c>
       <c r="D6" s="153"/>
       <c r="E6" s="153"/>
@@ -46502,10 +46507,10 @@
       <c r="A16" s="66"/>
       <c r="B16" s="219"/>
       <c r="C16" s="139" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
       <c r="D16" s="141" t="s">
-        <v>556</v>
+        <v>553</v>
       </c>
       <c r="E16" s="140" t="s">
         <v>266</v>
@@ -46520,10 +46525,10 @@
         <v>282</v>
       </c>
       <c r="I16" s="162" t="s">
-        <v>560</v>
+        <v>557</v>
       </c>
       <c r="J16" s="291" t="s">
-        <v>561</v>
+        <v>558</v>
       </c>
       <c r="K16" s="315"/>
       <c r="L16" s="316"/>
@@ -47992,7 +47997,7 @@
         <v>161</v>
       </c>
       <c r="C6" s="150" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="D6" s="153"/>
       <c r="E6" s="153"/>
@@ -48215,7 +48220,7 @@
         <v>335</v>
       </c>
       <c r="D16" s="141" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
       <c r="E16" s="140" t="s">
         <v>266</v>
@@ -49705,7 +49710,7 @@
         <v>161</v>
       </c>
       <c r="C6" s="150" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D6" s="153"/>
       <c r="E6" s="153"/>
@@ -49895,7 +49900,7 @@
         <v>338</v>
       </c>
       <c r="D15" s="141" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
       <c r="E15" s="140" t="s">
         <v>313</v>
@@ -51712,7 +51717,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:L61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
@@ -51938,7 +51943,7 @@
     </row>
     <row r="17" spans="2:8">
       <c r="B17" s="117" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
       <c r="C17" s="124"/>
       <c r="D17" s="124"/>
@@ -51964,7 +51969,7 @@
         <v>1</v>
       </c>
       <c r="C19" s="147" t="s">
-        <v>591</v>
+        <v>588</v>
       </c>
       <c r="D19" s="274" t="s">
         <v>4</v>
@@ -51979,10 +51984,10 @@
         <v>2</v>
       </c>
       <c r="C20" s="147" t="s">
-        <v>592</v>
+        <v>589</v>
       </c>
       <c r="D20" s="274" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
       <c r="E20" s="274"/>
       <c r="F20" s="148"/>
@@ -51994,7 +51999,7 @@
         <v>3</v>
       </c>
       <c r="C21" s="147" t="s">
-        <v>593</v>
+        <v>590</v>
       </c>
       <c r="D21" s="274" t="s">
         <v>24</v>
@@ -52009,7 +52014,7 @@
         <v>4</v>
       </c>
       <c r="C22" s="147" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
       <c r="D22" s="274" t="s">
         <v>5</v>
@@ -52024,7 +52029,7 @@
         <v>5</v>
       </c>
       <c r="C23" s="147" t="s">
-        <v>595</v>
+        <v>592</v>
       </c>
       <c r="D23" s="274" t="s">
         <v>26</v>
@@ -52039,7 +52044,7 @@
         <v>6</v>
       </c>
       <c r="C24" s="147" t="s">
-        <v>596</v>
+        <v>593</v>
       </c>
       <c r="D24" s="274" t="s">
         <v>25</v>
@@ -52095,7 +52100,7 @@
         <v>17</v>
       </c>
       <c r="D29" s="274" t="s">
-        <v>589</v>
+        <v>586</v>
       </c>
       <c r="E29" s="274"/>
       <c r="F29" s="148"/>
@@ -52110,7 +52115,7 @@
         <v>18</v>
       </c>
       <c r="D30" s="274" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="E30" s="274"/>
       <c r="F30" s="148"/>
@@ -52125,7 +52130,7 @@
         <v>19</v>
       </c>
       <c r="D31" s="274" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
       <c r="E31" s="274"/>
       <c r="F31" s="148"/>
@@ -52140,7 +52145,7 @@
         <v>20</v>
       </c>
       <c r="D32" s="274" t="s">
-        <v>609</v>
+        <v>606</v>
       </c>
       <c r="E32" s="274"/>
       <c r="F32" s="148"/>
@@ -52212,10 +52217,10 @@
         <v>10</v>
       </c>
       <c r="C37" s="147" t="s">
-        <v>614</v>
+        <v>611</v>
       </c>
       <c r="D37" s="274" t="s">
-        <v>616</v>
+        <v>613</v>
       </c>
       <c r="E37" s="274"/>
       <c r="F37" s="148"/>
@@ -52227,10 +52232,10 @@
         <v>11</v>
       </c>
       <c r="C38" s="147" t="s">
-        <v>615</v>
+        <v>612</v>
       </c>
       <c r="D38" s="274" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="E38" s="274"/>
       <c r="F38" s="148"/>
@@ -52242,10 +52247,10 @@
         <v>12</v>
       </c>
       <c r="C39" s="147" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="D39" s="274" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
       <c r="E39" s="274"/>
       <c r="F39" s="148"/>
@@ -52257,10 +52262,10 @@
         <v>13</v>
       </c>
       <c r="C40" s="147" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
       <c r="D40" s="274" t="s">
-        <v>624</v>
+        <v>621</v>
       </c>
       <c r="E40" s="274"/>
       <c r="F40" s="148"/>
@@ -52272,10 +52277,10 @@
         <v>14</v>
       </c>
       <c r="C41" s="147" t="s">
+        <v>622</v>
+      </c>
+      <c r="D41" s="274" t="s">
         <v>625</v>
-      </c>
-      <c r="D41" s="274" t="s">
-        <v>628</v>
       </c>
       <c r="E41" s="274"/>
       <c r="F41" s="148"/>
@@ -52287,10 +52292,10 @@
         <v>15</v>
       </c>
       <c r="C42" s="147" t="s">
+        <v>623</v>
+      </c>
+      <c r="D42" s="274" t="s">
         <v>626</v>
-      </c>
-      <c r="D42" s="274" t="s">
-        <v>629</v>
       </c>
       <c r="E42" s="274"/>
       <c r="F42" s="148"/>
@@ -52302,10 +52307,10 @@
         <v>16</v>
       </c>
       <c r="C43" s="147" t="s">
+        <v>624</v>
+      </c>
+      <c r="D43" s="274" t="s">
         <v>627</v>
-      </c>
-      <c r="D43" s="274" t="s">
-        <v>630</v>
       </c>
       <c r="E43" s="274"/>
       <c r="F43" s="148"/>
@@ -52547,8 +52552,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:N32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -52661,10 +52666,10 @@
         <v>514</v>
       </c>
       <c r="F6" s="102" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
       <c r="G6" s="102" t="s">
-        <v>611</v>
+        <v>608</v>
       </c>
       <c r="H6" s="103" t="s">
         <v>508</v>
@@ -52685,10 +52690,10 @@
         <v>514</v>
       </c>
       <c r="F7" s="102" t="s">
-        <v>618</v>
+        <v>615</v>
       </c>
       <c r="G7" s="102" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
       <c r="H7" s="103" t="s">
         <v>441</v>
@@ -52733,13 +52738,13 @@
         <v>464</v>
       </c>
       <c r="F9" s="211" t="s">
-        <v>534</v>
+        <v>531</v>
       </c>
       <c r="G9" s="101" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
       <c r="H9" s="103" t="s">
-        <v>547</v>
+        <v>544</v>
       </c>
       <c r="I9" s="104"/>
       <c r="J9" s="38"/>
@@ -52757,7 +52762,7 @@
         <v>464</v>
       </c>
       <c r="F10" s="211" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="G10" s="101" t="s">
         <v>515</v>
@@ -52781,10 +52786,10 @@
         <v>464</v>
       </c>
       <c r="F11" s="211" t="s">
-        <v>529</v>
+        <v>630</v>
       </c>
       <c r="G11" s="101" t="s">
-        <v>516</v>
+        <v>631</v>
       </c>
       <c r="H11" s="100" t="s">
         <v>505</v>
@@ -52821,7 +52826,7 @@
         <v>232</v>
       </c>
       <c r="G13" s="107" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
       <c r="H13" s="108" t="s">
         <v>238</v>
@@ -52866,10 +52871,10 @@
         <v>235</v>
       </c>
       <c r="F15" s="107" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="G15" s="107" t="s">
-        <v>545</v>
+        <v>542</v>
       </c>
       <c r="H15" s="108" t="s">
         <v>245</v>
@@ -52890,10 +52895,10 @@
         <v>231</v>
       </c>
       <c r="F16" s="107" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="G16" s="107" t="s">
-        <v>546</v>
+        <v>543</v>
       </c>
       <c r="H16" s="108" t="s">
         <v>244</v>
@@ -52914,10 +52919,10 @@
         <v>236</v>
       </c>
       <c r="F17" s="107" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="G17" s="107" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="H17" s="108" t="s">
         <v>246</v>
@@ -52938,10 +52943,10 @@
         <v>237</v>
       </c>
       <c r="F18" s="107" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="G18" s="107" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="H18" s="108" t="s">
         <v>247</v>
@@ -52977,10 +52982,10 @@
         <v>234</v>
       </c>
       <c r="F20" s="111" t="s">
+        <v>534</v>
+      </c>
+      <c r="G20" s="111" t="s">
         <v>537</v>
-      </c>
-      <c r="G20" s="111" t="s">
-        <v>540</v>
       </c>
       <c r="H20" s="112" t="s">
         <v>248</v>
@@ -53001,13 +53006,13 @@
         <v>239</v>
       </c>
       <c r="F21" s="111" t="s">
+        <v>535</v>
+      </c>
+      <c r="G21" s="111" t="s">
         <v>538</v>
       </c>
-      <c r="G21" s="111" t="s">
+      <c r="H21" s="112" t="s">
         <v>541</v>
-      </c>
-      <c r="H21" s="112" t="s">
-        <v>544</v>
       </c>
       <c r="I21" s="104"/>
       <c r="J21" s="38"/>
@@ -53025,10 +53030,10 @@
         <v>240</v>
       </c>
       <c r="F22" s="111" t="s">
+        <v>536</v>
+      </c>
+      <c r="G22" s="111" t="s">
         <v>539</v>
-      </c>
-      <c r="G22" s="111" t="s">
-        <v>542</v>
       </c>
       <c r="H22" s="112" t="s">
         <v>249</v>
@@ -53049,10 +53054,10 @@
         <v>241</v>
       </c>
       <c r="F23" s="111" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="G23" s="111" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
       <c r="H23" s="112" t="s">
         <v>250</v>
@@ -53319,7 +53324,7 @@
         <v>161</v>
       </c>
       <c r="C6" s="164" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="D6" s="172"/>
       <c r="E6" s="172"/>
@@ -53524,10 +53529,10 @@
         <v>50</v>
       </c>
       <c r="I15" s="158" t="s">
-        <v>563</v>
+        <v>560</v>
       </c>
       <c r="J15" s="304" t="s">
-        <v>562</v>
+        <v>559</v>
       </c>
       <c r="K15" s="304"/>
       <c r="L15" s="304"/>
@@ -53888,26 +53893,26 @@
       <c r="A27" s="168"/>
       <c r="B27" s="175"/>
       <c r="C27" s="139" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
       <c r="D27" s="141" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
       <c r="E27" s="140" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="F27" s="140"/>
       <c r="G27" s="140" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
       <c r="H27" s="140" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
       <c r="I27" s="158" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
       <c r="J27" s="164" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
       <c r="K27" s="172"/>
       <c r="L27" s="165"/>
@@ -54624,27 +54629,27 @@
       <c r="B54" s="184"/>
       <c r="C54" s="189"/>
       <c r="D54" s="217" t="s">
-        <v>564</v>
+        <v>561</v>
       </c>
       <c r="E54" s="216"/>
       <c r="F54" s="139" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
       <c r="G54" s="140" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
       <c r="H54" s="140"/>
       <c r="I54" s="140">
         <v>1</v>
       </c>
       <c r="J54" s="140" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
       <c r="K54" s="140" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
       <c r="L54" s="141" t="s">
-        <v>567</v>
+        <v>564</v>
       </c>
       <c r="M54" s="168"/>
       <c r="N54" s="168"/>
@@ -54655,24 +54660,24 @@
       <c r="B55" s="184"/>
       <c r="C55" s="189"/>
       <c r="D55" s="217" t="s">
-        <v>568</v>
+        <v>565</v>
       </c>
       <c r="E55" s="216"/>
       <c r="F55" s="139" t="s">
-        <v>582</v>
+        <v>579</v>
       </c>
       <c r="G55" s="140" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
       <c r="H55" s="140"/>
       <c r="I55" s="140">
         <v>1</v>
       </c>
       <c r="J55" s="140" t="s">
+        <v>563</v>
+      </c>
+      <c r="K55" s="140" t="s">
         <v>566</v>
-      </c>
-      <c r="K55" s="140" t="s">
-        <v>569</v>
       </c>
       <c r="L55" s="218" t="s">
         <v>411</v>
@@ -55817,7 +55822,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O106"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M30" sqref="M30"/>
     </sheetView>
   </sheetViews>
@@ -55943,7 +55948,7 @@
         <v>161</v>
       </c>
       <c r="C6" s="164" t="s">
-        <v>612</v>
+        <v>609</v>
       </c>
       <c r="D6" s="172"/>
       <c r="E6" s="172"/>
@@ -55964,7 +55969,7 @@
         <v>170</v>
       </c>
       <c r="C7" s="291" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="D7" s="299"/>
       <c r="E7" s="299"/>
@@ -55985,7 +55990,7 @@
         <v>171</v>
       </c>
       <c r="C8" s="164" t="s">
-        <v>613</v>
+        <v>610</v>
       </c>
       <c r="D8" s="172"/>
       <c r="E8" s="172"/>
@@ -57151,27 +57156,27 @@
       <c r="B51" s="184"/>
       <c r="C51" s="189"/>
       <c r="D51" s="217" t="s">
-        <v>564</v>
+        <v>561</v>
       </c>
       <c r="E51" s="216"/>
       <c r="F51" s="139" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
       <c r="G51" s="140" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
       <c r="H51" s="140"/>
       <c r="I51" s="140">
         <v>1</v>
       </c>
       <c r="J51" s="140" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
       <c r="K51" s="140" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
       <c r="L51" s="141" t="s">
-        <v>567</v>
+        <v>564</v>
       </c>
       <c r="M51" s="168"/>
       <c r="N51" s="168"/>
@@ -57182,24 +57187,24 @@
       <c r="B52" s="192"/>
       <c r="C52" s="190"/>
       <c r="D52" s="217" t="s">
-        <v>568</v>
+        <v>565</v>
       </c>
       <c r="E52" s="216"/>
       <c r="F52" s="139" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
       <c r="G52" s="140" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
       <c r="H52" s="140"/>
       <c r="I52" s="140">
         <v>1</v>
       </c>
       <c r="J52" s="140" t="s">
+        <v>563</v>
+      </c>
+      <c r="K52" s="140" t="s">
         <v>566</v>
-      </c>
-      <c r="K52" s="140" t="s">
-        <v>569</v>
       </c>
       <c r="L52" s="218" t="s">
         <v>411</v>
@@ -58305,7 +58310,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O78"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A34" workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -58431,7 +58436,7 @@
         <v>161</v>
       </c>
       <c r="C6" s="164" t="s">
-        <v>620</v>
+        <v>617</v>
       </c>
       <c r="D6" s="172"/>
       <c r="E6" s="172"/>
@@ -58452,7 +58457,7 @@
         <v>170</v>
       </c>
       <c r="C7" s="291" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="D7" s="299"/>
       <c r="E7" s="299"/>
@@ -60343,7 +60348,7 @@
         <v>50</v>
       </c>
       <c r="I15" s="158" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="J15" s="164" t="s">
         <v>457</v>
@@ -60939,14 +60944,14 @@
       <c r="B38" s="192"/>
       <c r="C38" s="190"/>
       <c r="D38" s="291" t="s">
-        <v>570</v>
+        <v>567</v>
       </c>
       <c r="E38" s="290"/>
       <c r="F38" s="139" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
       <c r="G38" s="140" t="s">
-        <v>572</v>
+        <v>569</v>
       </c>
       <c r="H38" s="140" t="s">
         <v>185</v>
@@ -60955,13 +60960,13 @@
         <v>1</v>
       </c>
       <c r="J38" s="140" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
       <c r="K38" s="140" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
       <c r="L38" s="141" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
       <c r="M38" s="168"/>
       <c r="N38" s="168"/>

</xml_diff>